<commit_message>
completed witch single NG
</commit_message>
<xml_diff>
--- a/DeliveryDateSpec (1).xlsx
+++ b/DeliveryDateSpec (1).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="72">
   <si>
     <t>指定希望納期</t>
     <rPh sb="0" eb="2">
@@ -384,10 +384,7 @@
     <t>Ok</t>
   </si>
   <si>
-    <t>check(29)</t>
-  </si>
-  <si>
-    <t>check(01)</t>
+    <t>NG(01)[check case]</t>
   </si>
 </sst>
 </file>
@@ -1508,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1848,7 +1845,7 @@
         <v>48</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>69</v>
@@ -1888,10 +1885,10 @@
         <v>48</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="2:7">
@@ -1911,7 +1908,7 @@
         <v>69</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="2:7">
@@ -1951,7 +1948,7 @@
         <v>69</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="2:7">
@@ -1967,6 +1964,12 @@
       <c r="E24" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="F24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="3" t="s">
@@ -1981,6 +1984,12 @@
       <c r="E25" t="s">
         <v>61</v>
       </c>
+      <c r="F25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="26" spans="2:7">
       <c r="B26" s="3" t="s">
@@ -1995,6 +2004,12 @@
       <c r="E26" t="s">
         <v>61</v>
       </c>
+      <c r="F26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="28" spans="2:7">
       <c r="B28" s="3" t="s">
@@ -2009,6 +2024,12 @@
       <c r="E28" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="F28" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="29" spans="2:7">
       <c r="B29" s="3" t="s">
@@ -2023,6 +2044,12 @@
       <c r="E29" t="s">
         <v>61</v>
       </c>
+      <c r="F29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="30" spans="2:7">
       <c r="B30" s="3" t="s">
@@ -2037,6 +2064,12 @@
       <c r="E30" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="F30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="31" spans="2:7">
       <c r="B31" s="3" t="s">
@@ -2051,6 +2084,12 @@
       <c r="E31" t="s">
         <v>61</v>
       </c>
+      <c r="F31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="32" spans="2:7">
       <c r="B32" s="3" t="s">
@@ -2065,6 +2104,12 @@
       <c r="E32" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="F32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="33" spans="2:7">
       <c r="B33" s="3" t="s">
@@ -2079,6 +2124,12 @@
       <c r="E33" t="s">
         <v>61</v>
       </c>
+      <c r="F33" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="34" spans="2:7">
       <c r="B34" s="3" t="s">
@@ -2093,6 +2144,12 @@
       <c r="E34" t="s">
         <v>61</v>
       </c>
+      <c r="F34" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="35" spans="2:7">
       <c r="B35" s="3" t="s">
@@ -2107,6 +2164,12 @@
       <c r="E35" t="s">
         <v>61</v>
       </c>
+      <c r="F35" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="37" spans="2:7">
       <c r="B37" s="3" t="s">
@@ -2141,6 +2204,12 @@
       <c r="E38" t="s">
         <v>62</v>
       </c>
+      <c r="F38" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="39" spans="2:7">
       <c r="B39" s="3" t="s">
@@ -2155,8 +2224,12 @@
       <c r="E39" t="s">
         <v>61</v>
       </c>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
+      <c r="F39" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="40" spans="2:7">
       <c r="B40" s="3" t="s">
@@ -2171,6 +2244,12 @@
       <c r="E40" t="s">
         <v>62</v>
       </c>
+      <c r="F40" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="41" spans="2:7">
       <c r="B41" s="3" t="s">
@@ -2185,6 +2264,12 @@
       <c r="E41" t="s">
         <v>62</v>
       </c>
+      <c r="F41" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="42" spans="2:7">
       <c r="B42" s="3" t="s">
@@ -2199,6 +2284,12 @@
       <c r="E42" t="s">
         <v>62</v>
       </c>
+      <c r="F42" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="43" spans="2:7">
       <c r="B43" s="3" t="s">
@@ -2213,6 +2304,12 @@
       <c r="E43" t="s">
         <v>61</v>
       </c>
+      <c r="F43" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="44" spans="2:7">
       <c r="B44" s="3" t="s">
@@ -2227,6 +2324,12 @@
       <c r="E44" t="s">
         <v>62</v>
       </c>
+      <c r="F44" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="46" spans="2:7">
       <c r="B46" s="3" t="s">
@@ -2241,10 +2344,10 @@
       <c r="E46" t="s">
         <v>63</v>
       </c>
-      <c r="F46" t="s">
-        <v>70</v>
-      </c>
-      <c r="G46" t="s">
+      <c r="F46" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2261,10 +2364,10 @@
       <c r="E47" t="s">
         <v>63</v>
       </c>
-      <c r="F47" t="s">
-        <v>69</v>
-      </c>
-      <c r="G47" t="s">
+      <c r="F47" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G47" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2281,10 +2384,10 @@
       <c r="E48" t="s">
         <v>63</v>
       </c>
-      <c r="F48" t="s">
-        <v>69</v>
-      </c>
-      <c r="G48" t="s">
+      <c r="F48" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2301,10 +2404,10 @@
       <c r="E49" t="s">
         <v>63</v>
       </c>
-      <c r="F49" t="s">
-        <v>69</v>
-      </c>
-      <c r="G49" t="s">
+      <c r="F49" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G49" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2321,10 +2424,10 @@
       <c r="E50" t="s">
         <v>63</v>
       </c>
-      <c r="F50" t="s">
-        <v>69</v>
-      </c>
-      <c r="G50" t="s">
+      <c r="F50" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2341,10 +2444,10 @@
       <c r="E51" t="s">
         <v>63</v>
       </c>
-      <c r="F51" t="s">
-        <v>69</v>
-      </c>
-      <c r="G51" t="s">
+      <c r="F51" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2361,10 +2464,10 @@
       <c r="E53" t="s">
         <v>63</v>
       </c>
-      <c r="F53" t="s">
-        <v>69</v>
-      </c>
-      <c r="G53" t="s">
+      <c r="F53" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G53" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2381,10 +2484,10 @@
       <c r="E54" t="s">
         <v>63</v>
       </c>
-      <c r="F54" t="s">
-        <v>69</v>
-      </c>
-      <c r="G54" t="s">
+      <c r="F54" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G54" s="3" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>